<commit_message>
Avances en la Bitácora
</commit_message>
<xml_diff>
--- a/Bitácora.xlsx
+++ b/Bitácora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Documents\Universidad\8vo Semestre\Lab. Computación Gráfica\Proyecto_Final_Computacion_Grafica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049B6DFD-F46E-4101-8B9B-3FE5455FAD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68094FB-DAE3-4170-8AE3-35657E7CC15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10653" yWindow="5540" windowWidth="19200" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>